<commit_message>
Izbrisani p pri sifrah - NAROBE VPISALI
</commit_message>
<xml_diff>
--- a/products/Seznam_artiklov_Sifrant_magnet_kovinski_ok.xlsx
+++ b/products/Seznam_artiklov_Sifrant_magnet_kovinski_ok.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aljaz\Desktop\Aljaz\Trafika main\trafika\products\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{2B71B150-3FFB-470F-B817-8ADE0604FD20}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="120" yWindow="156" windowWidth="20112" windowHeight="7992" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -759,96 +765,42 @@
     <t>Ljubljana_ladjica</t>
   </si>
   <si>
-    <t>MAG135p</t>
-  </si>
-  <si>
     <t>Piran_punta</t>
   </si>
   <si>
     <t>pravokotnik 115x40mm</t>
   </si>
   <si>
-    <t>MAG136p</t>
-  </si>
-  <si>
-    <t>MAG137p</t>
-  </si>
-  <si>
-    <t>MAG138p</t>
-  </si>
-  <si>
-    <t>MAG139p</t>
-  </si>
-  <si>
-    <t>MAG140p</t>
-  </si>
-  <si>
     <t>Ljubljana - zmaj_nočna_ladjica</t>
   </si>
   <si>
     <t>Ljubljana, zmaj, nočna, ladjica</t>
   </si>
   <si>
-    <t>MAG141p</t>
-  </si>
-  <si>
-    <t>MAG142p</t>
-  </si>
-  <si>
     <t>Ljubljana_tržnica_Plečnik</t>
   </si>
   <si>
     <t>Ljubljana, tržnica, Plečnik</t>
   </si>
   <si>
-    <t>MAG143p</t>
-  </si>
-  <si>
-    <t>MAG144p</t>
-  </si>
-  <si>
     <t>Kranjska gora</t>
   </si>
   <si>
     <t>Kranjska gora, Gorenjska</t>
   </si>
   <si>
-    <t>MAG145p</t>
-  </si>
-  <si>
-    <t>MAG146p</t>
-  </si>
-  <si>
     <t>Postojnska jama_pokončna</t>
   </si>
   <si>
-    <t>MAG147p</t>
-  </si>
-  <si>
-    <t>MAG148p</t>
-  </si>
-  <si>
-    <t>MAG149p</t>
-  </si>
-  <si>
-    <t>MAG150p</t>
-  </si>
-  <si>
     <t>Bled_grad_otok_pokončna</t>
   </si>
   <si>
     <t>Bled, grad, otok, Gorenjska</t>
   </si>
   <si>
-    <t>MAG151p</t>
-  </si>
-  <si>
     <t>Zmajski most_večerna</t>
   </si>
   <si>
-    <t>MAG152p</t>
-  </si>
-  <si>
     <t>MAG153</t>
   </si>
   <si>
@@ -936,84 +888,51 @@
     <t>Predjamski grad, Postojnska jama</t>
   </si>
   <si>
-    <t>MAG167p</t>
-  </si>
-  <si>
     <t>Slovenija - zmaj_Bled_Piran</t>
   </si>
   <si>
     <t>Slovenija, zmaj, Bled, Piran, Gorenjska, Obala</t>
   </si>
   <si>
-    <t>MAG168p</t>
-  </si>
-  <si>
-    <t>MAG169p</t>
-  </si>
-  <si>
     <t>Slovenija - Postojnska jama_Lipica_Predjamski grad</t>
   </si>
   <si>
     <t>Slovenija, Postojnska jama, Lipica, Predjamski grad</t>
   </si>
   <si>
-    <t>MAG170p</t>
-  </si>
-  <si>
     <t>Slovenija - Ljubljana_Tromostovje_Zmajski most</t>
   </si>
   <si>
     <t>Slovenija, Ljubljana, Tromostovje, Zmajski most</t>
   </si>
   <si>
-    <t>MAG171p</t>
-  </si>
-  <si>
     <t>Slovenija - Zmajski most_ stolnica_ladjica</t>
   </si>
   <si>
     <t>Slovenija, Zmajski most,  stolnica, ladjica</t>
   </si>
   <si>
-    <t>MAG172p</t>
-  </si>
-  <si>
     <t>Slovenija - Piran_Lipica_Bled_Postojnska jama_Ljubljana_pokončna</t>
   </si>
   <si>
     <t>Slovenija, Piran, Lipica, Bled, Postojnska jama, Ljubljana, Gorenjska, Obala</t>
   </si>
   <si>
-    <t>MAG173p</t>
-  </si>
-  <si>
     <t>Bovec - raft_Bovec panorama_korita Soče</t>
   </si>
   <si>
     <t>Bovec, raft, korita Soče, Dolina Soče</t>
   </si>
   <si>
-    <t>MAG174p</t>
-  </si>
-  <si>
     <t>Slovenija - Ljubljana panorama_Tromostovje_Zmajski most_bel rob</t>
   </si>
   <si>
-    <t>MAG175p</t>
-  </si>
-  <si>
     <t>Slovenija - Ljubljana_Postojnska jama_Piran_Bled_bel rob</t>
   </si>
   <si>
-    <t>MAG176p</t>
-  </si>
-  <si>
     <t>Bled_srce parček</t>
   </si>
   <si>
-    <t>MAG177p</t>
-  </si>
-  <si>
     <t>Ljubljana_srce parček</t>
   </si>
   <si>
@@ -1089,36 +1008,21 @@
     <t>Ajdovska deklica, Vršič, Gorenjska, Dolina Soče</t>
   </si>
   <si>
-    <t>MAG187p</t>
-  </si>
-  <si>
     <t>Vršič, Gorenjska, Dolina Soče</t>
   </si>
   <si>
-    <t>MAG188p</t>
-  </si>
-  <si>
     <t>Slovenija - Ruska kapelica_Vršič_Ajdovska deklica</t>
   </si>
   <si>
     <t>Slovenija, Ruska kapelica, Vršič, Ajdovska deklica, Gorenjska, Dolina Soče</t>
   </si>
   <si>
-    <t>MAG189p</t>
-  </si>
-  <si>
     <t>Slovenija - Krn_Kobarid(kostnica)_Soča</t>
   </si>
   <si>
     <t>Slovenija, Krn, Kobarid, kostnica, Soča, Dolina Soče</t>
   </si>
   <si>
-    <t>MAG190p</t>
-  </si>
-  <si>
-    <t>MAG191p</t>
-  </si>
-  <si>
     <t>Ljubljana_panorama_zimska</t>
   </si>
   <si>
@@ -1159,12 +1063,114 @@
   </si>
   <si>
     <t>Šifrant magnet_kovinski</t>
+  </si>
+  <si>
+    <t>MAG167</t>
+  </si>
+  <si>
+    <t>MAG168</t>
+  </si>
+  <si>
+    <t>MAG169</t>
+  </si>
+  <si>
+    <t>MAG170</t>
+  </si>
+  <si>
+    <t>MAG171</t>
+  </si>
+  <si>
+    <t>MAG172</t>
+  </si>
+  <si>
+    <t>MAG173</t>
+  </si>
+  <si>
+    <t>MAG174</t>
+  </si>
+  <si>
+    <t>MAG175</t>
+  </si>
+  <si>
+    <t>MAG176</t>
+  </si>
+  <si>
+    <t>MAG177</t>
+  </si>
+  <si>
+    <t>MAG187</t>
+  </si>
+  <si>
+    <t>MAG188</t>
+  </si>
+  <si>
+    <t>MAG189</t>
+  </si>
+  <si>
+    <t>MAG190</t>
+  </si>
+  <si>
+    <t>MAG191</t>
+  </si>
+  <si>
+    <t>MAG135</t>
+  </si>
+  <si>
+    <t>MAG136</t>
+  </si>
+  <si>
+    <t>MAG137</t>
+  </si>
+  <si>
+    <t>MAG138</t>
+  </si>
+  <si>
+    <t>MAG139</t>
+  </si>
+  <si>
+    <t>MAG140</t>
+  </si>
+  <si>
+    <t>MAG141</t>
+  </si>
+  <si>
+    <t>MAG142</t>
+  </si>
+  <si>
+    <t>MAG143</t>
+  </si>
+  <si>
+    <t>MAG144</t>
+  </si>
+  <si>
+    <t>MAG145</t>
+  </si>
+  <si>
+    <t>MAG146</t>
+  </si>
+  <si>
+    <t>MAG147</t>
+  </si>
+  <si>
+    <t>MAG148</t>
+  </si>
+  <si>
+    <t>MAG149</t>
+  </si>
+  <si>
+    <t>MAG150</t>
+  </si>
+  <si>
+    <t>MAG151</t>
+  </si>
+  <si>
+    <t>MAG152</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1497,24 +1503,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Excel Built-in Normal" xfId="1"/>
+    <cellStyle name="Excel Built-in Normal" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Navadno" xfId="0" builtinId="0"/>
-    <cellStyle name="Navadno 2" xfId="2"/>
-    <cellStyle name="Navadno 4" xfId="3"/>
+    <cellStyle name="Navadno 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Navadno 4" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1563,7 +1572,7 @@
     </a:clrScheme>
     <a:fontScheme name="Pisarna">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1596,9 +1605,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1631,6 +1657,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Pisarna">
@@ -1806,32 +1849,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:G165"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B115" sqref="B115"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.5703125" style="9" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" style="31" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" style="34" customWidth="1"/>
-    <col min="4" max="4" width="58.7109375" style="47" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" style="31" customWidth="1"/>
-    <col min="6" max="6" width="24.140625" style="34" customWidth="1"/>
-    <col min="7" max="7" width="67.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.5546875" style="9" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" style="31" customWidth="1"/>
+    <col min="3" max="3" width="19.88671875" style="34" customWidth="1"/>
+    <col min="4" max="4" width="58.6640625" style="47" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" style="31" customWidth="1"/>
+    <col min="6" max="6" width="24.109375" style="34" customWidth="1"/>
+    <col min="7" max="7" width="67.109375" style="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="50" t="s">
-        <v>380</v>
-      </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-    </row>
-    <row r="4" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.3">
+      <c r="A2" s="49" t="s">
+        <v>346</v>
+      </c>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+    </row>
+    <row r="4" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>0</v>
       </c>
@@ -1854,7 +1897,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="15"/>
       <c r="B5" s="35" t="s">
         <v>7</v>
@@ -1875,7 +1918,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="17"/>
       <c r="B6" s="36" t="s">
         <v>12</v>
@@ -1896,7 +1939,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="37" t="s">
         <v>15</v>
@@ -1917,7 +1960,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="17"/>
       <c r="B8" s="36" t="s">
         <v>18</v>
@@ -1938,7 +1981,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="17"/>
       <c r="B9" s="36" t="s">
         <v>21</v>
@@ -1959,7 +2002,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="17"/>
       <c r="B10" s="36" t="s">
         <v>24</v>
@@ -1980,7 +2023,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="17"/>
       <c r="B11" s="36" t="s">
         <v>26</v>
@@ -2001,7 +2044,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="17"/>
       <c r="B12" s="36" t="s">
         <v>29</v>
@@ -2022,7 +2065,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="17"/>
       <c r="B13" s="36" t="s">
         <v>32</v>
@@ -2043,7 +2086,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="B14" s="37" t="s">
         <v>34</v>
@@ -2064,7 +2107,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="17"/>
       <c r="B15" s="36" t="s">
         <v>36</v>
@@ -2085,7 +2128,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="17"/>
       <c r="B16" s="36" t="s">
         <v>38</v>
@@ -2106,7 +2149,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="17"/>
       <c r="B17" s="36" t="s">
         <v>41</v>
@@ -2127,7 +2170,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="17"/>
       <c r="B18" s="36" t="s">
         <v>44</v>
@@ -2148,7 +2191,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
       <c r="B19" s="37" t="s">
         <v>46</v>
@@ -2169,7 +2212,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="17"/>
       <c r="B20" s="36" t="s">
         <v>49</v>
@@ -2190,7 +2233,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="17"/>
       <c r="B21" s="36" t="s">
         <v>52</v>
@@ -2211,7 +2254,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="17"/>
       <c r="B22" s="36" t="s">
         <v>55</v>
@@ -2232,7 +2275,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="17"/>
       <c r="B23" s="36" t="s">
         <v>58</v>
@@ -2253,7 +2296,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="17"/>
       <c r="B24" s="36" t="s">
         <v>60</v>
@@ -2274,7 +2317,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="17"/>
       <c r="B25" s="36" t="s">
         <v>62</v>
@@ -2295,7 +2338,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="26" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="17"/>
       <c r="B26" s="36" t="s">
         <v>65</v>
@@ -2316,7 +2359,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="27" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="17"/>
       <c r="B27" s="36" t="s">
         <v>67</v>
@@ -2337,7 +2380,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="17"/>
       <c r="B28" s="36" t="s">
         <v>70</v>
@@ -2358,7 +2401,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="17"/>
       <c r="B29" s="36" t="s">
         <v>72</v>
@@ -2379,7 +2422,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="30" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="17"/>
       <c r="B30" s="36" t="s">
         <v>75</v>
@@ -2400,7 +2443,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="31" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="17"/>
       <c r="B31" s="36" t="s">
         <v>78</v>
@@ -2421,7 +2464,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="32" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="17"/>
       <c r="B32" s="36" t="s">
         <v>81</v>
@@ -2442,7 +2485,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="33" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="17"/>
       <c r="B33" s="36" t="s">
         <v>84</v>
@@ -2463,7 +2506,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="34" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="17"/>
       <c r="B34" s="36" t="s">
         <v>87</v>
@@ -2484,7 +2527,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="35" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="17"/>
       <c r="B35" s="36" t="s">
         <v>90</v>
@@ -2505,7 +2548,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="36" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="17"/>
       <c r="B36" s="36" t="s">
         <v>93</v>
@@ -2526,7 +2569,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="37" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="17"/>
       <c r="B37" s="36" t="s">
         <v>96</v>
@@ -2547,7 +2590,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="38" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="17"/>
       <c r="B38" s="36" t="s">
         <v>99</v>
@@ -2568,7 +2611,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="39" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="17"/>
       <c r="B39" s="36" t="s">
         <v>102</v>
@@ -2589,7 +2632,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="40" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="17"/>
       <c r="B40" s="36" t="s">
         <v>105</v>
@@ -2610,7 +2653,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="41" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="17"/>
       <c r="B41" s="36" t="s">
         <v>108</v>
@@ -2631,7 +2674,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="42" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="17"/>
       <c r="B42" s="36" t="s">
         <v>111</v>
@@ -2652,7 +2695,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="43" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="17"/>
       <c r="B43" s="36" t="s">
         <v>112</v>
@@ -2673,7 +2716,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="44" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="17"/>
       <c r="B44" s="36" t="s">
         <v>114</v>
@@ -2694,7 +2737,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="45" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="2"/>
       <c r="B45" s="37" t="s">
         <v>116</v>
@@ -2715,7 +2758,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="46" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="2"/>
       <c r="B46" s="37" t="s">
         <v>119</v>
@@ -2736,7 +2779,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="47" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="2"/>
       <c r="B47" s="37" t="s">
         <v>122</v>
@@ -2757,7 +2800,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="48" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="17"/>
       <c r="B48" s="36" t="s">
         <v>124</v>
@@ -2778,7 +2821,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="49" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="17"/>
       <c r="B49" s="36" t="s">
         <v>127</v>
@@ -2799,7 +2842,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="50" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="17"/>
       <c r="B50" s="36" t="s">
         <v>130</v>
@@ -2820,7 +2863,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="51" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="17"/>
       <c r="B51" s="36" t="s">
         <v>131</v>
@@ -2841,7 +2884,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="52" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="17"/>
       <c r="B52" s="36" t="s">
         <v>134</v>
@@ -2862,7 +2905,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="53" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="17"/>
       <c r="B53" s="36" t="s">
         <v>136</v>
@@ -2883,7 +2926,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="54" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A54" s="17"/>
       <c r="B54" s="36" t="s">
         <v>138</v>
@@ -2904,7 +2947,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="55" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A55" s="17"/>
       <c r="B55" s="36" t="s">
         <v>141</v>
@@ -2925,7 +2968,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="56" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="17"/>
       <c r="B56" s="36" t="s">
         <v>144</v>
@@ -2946,7 +2989,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="57" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57" s="17"/>
       <c r="B57" s="36" t="s">
         <v>147</v>
@@ -2967,7 +3010,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="58" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="17"/>
       <c r="B58" s="36" t="s">
         <v>149</v>
@@ -2988,7 +3031,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="59" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A59" s="17"/>
       <c r="B59" s="36" t="s">
         <v>152</v>
@@ -3009,7 +3052,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="60" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="17"/>
       <c r="B60" s="36" t="s">
         <v>155</v>
@@ -3030,7 +3073,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="61" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A61" s="17"/>
       <c r="B61" s="36" t="s">
         <v>158</v>
@@ -3051,7 +3094,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="62" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A62" s="17"/>
       <c r="B62" s="36" t="s">
         <v>161</v>
@@ -3072,7 +3115,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="63" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A63" s="17"/>
       <c r="B63" s="36" t="s">
         <v>163</v>
@@ -3093,7 +3136,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="64" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A64" s="17"/>
       <c r="B64" s="36" t="s">
         <v>165</v>
@@ -3114,7 +3157,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="65" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A65" s="17"/>
       <c r="B65" s="36" t="s">
         <v>167</v>
@@ -3135,7 +3178,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="66" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A66" s="17"/>
       <c r="B66" s="36" t="s">
         <v>169</v>
@@ -3156,7 +3199,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="67" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A67" s="17"/>
       <c r="B67" s="36" t="s">
         <v>171</v>
@@ -3177,7 +3220,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="68" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A68" s="17"/>
       <c r="B68" s="36" t="s">
         <v>173</v>
@@ -3198,7 +3241,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="69" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A69" s="17"/>
       <c r="B69" s="36" t="s">
         <v>176</v>
@@ -3219,7 +3262,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="70" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A70" s="17"/>
       <c r="B70" s="36" t="s">
         <v>179</v>
@@ -3240,7 +3283,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="71" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A71" s="17"/>
       <c r="B71" s="36" t="s">
         <v>181</v>
@@ -3261,7 +3304,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="72" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A72" s="17"/>
       <c r="B72" s="36" t="s">
         <v>184</v>
@@ -3282,7 +3325,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="73" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A73" s="17"/>
       <c r="B73" s="36" t="s">
         <v>186</v>
@@ -3303,7 +3346,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="74" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A74" s="17"/>
       <c r="B74" s="36" t="s">
         <v>189</v>
@@ -3324,7 +3367,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="75" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A75" s="17"/>
       <c r="B75" s="36" t="s">
         <v>192</v>
@@ -3342,10 +3385,10 @@
         <v>10</v>
       </c>
       <c r="G75" s="21" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A76" s="17"/>
       <c r="B76" s="36" t="s">
         <v>194</v>
@@ -3366,7 +3409,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="77" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A77" s="17"/>
       <c r="B77" s="36" t="s">
         <v>197</v>
@@ -3387,7 +3430,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="78" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A78" s="17"/>
       <c r="B78" s="36" t="s">
         <v>199</v>
@@ -3405,10 +3448,10 @@
         <v>10</v>
       </c>
       <c r="G78" s="21" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A79" s="17"/>
       <c r="B79" s="36" t="s">
         <v>201</v>
@@ -3429,7 +3472,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="80" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A80" s="17"/>
       <c r="B80" s="36" t="s">
         <v>202</v>
@@ -3450,7 +3493,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="81" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A81" s="17"/>
       <c r="B81" s="36" t="s">
         <v>205</v>
@@ -3471,7 +3514,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="82" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A82" s="17"/>
       <c r="B82" s="36" t="s">
         <v>208</v>
@@ -3492,7 +3535,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="83" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A83" s="17"/>
       <c r="B83" s="36" t="s">
         <v>211</v>
@@ -3513,7 +3556,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="84" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A84" s="17"/>
       <c r="B84" s="36" t="s">
         <v>214</v>
@@ -3534,7 +3577,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="85" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A85" s="17"/>
       <c r="B85" s="36" t="s">
         <v>217</v>
@@ -3555,7 +3598,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="86" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A86" s="17"/>
       <c r="B86" s="36" t="s">
         <v>220</v>
@@ -3576,7 +3619,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="87" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A87" s="17"/>
       <c r="B87" s="36" t="s">
         <v>223</v>
@@ -3597,7 +3640,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="88" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A88" s="17"/>
       <c r="B88" s="36" t="s">
         <v>226</v>
@@ -3618,7 +3661,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="89" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A89" s="17"/>
       <c r="B89" s="36" t="s">
         <v>229</v>
@@ -3639,7 +3682,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="90" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A90" s="3"/>
       <c r="B90" s="39" t="s">
         <v>232</v>
@@ -3660,7 +3703,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="91" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A91" s="3"/>
       <c r="B91" s="39" t="s">
         <v>234</v>
@@ -3681,7 +3724,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="92" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A92" s="3"/>
       <c r="B92" s="39" t="s">
         <v>236</v>
@@ -3702,7 +3745,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="93" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A93" s="3"/>
       <c r="B93" s="39" t="s">
         <v>238</v>
@@ -3723,7 +3766,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="94" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A94" s="3"/>
       <c r="B94" s="39" t="s">
         <v>239</v>
@@ -3744,7 +3787,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="95" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A95" s="3"/>
       <c r="B95" s="39" t="s">
         <v>240</v>
@@ -3765,7 +3808,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="96" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A96" s="3"/>
       <c r="B96" s="39" t="s">
         <v>242</v>
@@ -3786,7 +3829,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="97" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A97" s="3"/>
       <c r="B97" s="39" t="s">
         <v>245</v>
@@ -3807,31 +3850,31 @@
         <v>69</v>
       </c>
     </row>
-    <row r="98" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A98" s="3"/>
       <c r="B98" s="39" t="s">
+        <v>363</v>
+      </c>
+      <c r="C98" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="D98" s="39" t="s">
         <v>247</v>
       </c>
-      <c r="C98" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="D98" s="39" t="s">
+      <c r="E98" s="28">
+        <v>3830008640413</v>
+      </c>
+      <c r="F98" s="29" t="s">
         <v>248</v>
-      </c>
-      <c r="E98" s="28">
-        <v>3830008640413</v>
-      </c>
-      <c r="F98" s="29" t="s">
-        <v>249</v>
       </c>
       <c r="G98" s="21" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="99" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A99" s="3"/>
       <c r="B99" s="39" t="s">
-        <v>250</v>
+        <v>364</v>
       </c>
       <c r="C99" s="35" t="s">
         <v>8</v>
@@ -3843,16 +3886,16 @@
         <v>3830008640413</v>
       </c>
       <c r="F99" s="29" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G99" s="21" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="100" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A100" s="3"/>
       <c r="B100" s="39" t="s">
-        <v>251</v>
+        <v>365</v>
       </c>
       <c r="C100" s="35" t="s">
         <v>8</v>
@@ -3864,16 +3907,16 @@
         <v>3830008640413</v>
       </c>
       <c r="F100" s="29" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G100" s="21" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="101" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A101" s="3"/>
       <c r="B101" s="39" t="s">
-        <v>252</v>
+        <v>366</v>
       </c>
       <c r="C101" s="35" t="s">
         <v>8</v>
@@ -3885,16 +3928,16 @@
         <v>3830008640413</v>
       </c>
       <c r="F101" s="29" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G101" s="21" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="102" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A102" s="3"/>
       <c r="B102" s="39" t="s">
-        <v>253</v>
+        <v>367</v>
       </c>
       <c r="C102" s="35" t="s">
         <v>8</v>
@@ -3906,37 +3949,37 @@
         <v>3830008640413</v>
       </c>
       <c r="F102" s="29" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G102" s="21" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="103" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A103" s="3"/>
       <c r="B103" s="39" t="s">
-        <v>254</v>
+        <v>368</v>
       </c>
       <c r="C103" s="35" t="s">
         <v>8</v>
       </c>
       <c r="D103" s="39" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="E103" s="28">
         <v>3830008640413</v>
       </c>
       <c r="F103" s="29" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G103" s="21" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A104" s="3"/>
       <c r="B104" s="39" t="s">
-        <v>257</v>
+        <v>369</v>
       </c>
       <c r="C104" s="35" t="s">
         <v>8</v>
@@ -3948,37 +3991,37 @@
         <v>3830008640413</v>
       </c>
       <c r="F104" s="29" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G104" s="21" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="105" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A105" s="3"/>
       <c r="B105" s="39" t="s">
-        <v>258</v>
+        <v>370</v>
       </c>
       <c r="C105" s="35" t="s">
         <v>8</v>
       </c>
       <c r="D105" s="39" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="E105" s="28">
         <v>3830008640413</v>
       </c>
       <c r="F105" s="29" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G105" s="21" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A106" s="2"/>
       <c r="B106" s="37" t="s">
-        <v>261</v>
+        <v>371</v>
       </c>
       <c r="C106" s="35" t="s">
         <v>8</v>
@@ -3990,37 +4033,37 @@
         <v>3830008640413</v>
       </c>
       <c r="F106" s="29" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G106" s="19" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="107" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A107" s="2"/>
       <c r="B107" s="37" t="s">
-        <v>262</v>
+        <v>372</v>
       </c>
       <c r="C107" s="35" t="s">
         <v>8</v>
       </c>
       <c r="D107" s="37" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="E107" s="28">
         <v>3830008640413</v>
       </c>
       <c r="F107" s="29" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G107" s="19" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A108" s="2"/>
       <c r="B108" s="37" t="s">
-        <v>265</v>
+        <v>373</v>
       </c>
       <c r="C108" s="35" t="s">
         <v>8</v>
@@ -4032,37 +4075,37 @@
         <v>3830008640413</v>
       </c>
       <c r="F108" s="29" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G108" s="19" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="109" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A109" s="3"/>
       <c r="B109" s="39" t="s">
-        <v>266</v>
+        <v>374</v>
       </c>
       <c r="C109" s="35" t="s">
         <v>8</v>
       </c>
       <c r="D109" s="39" t="s">
-        <v>267</v>
+        <v>255</v>
       </c>
       <c r="E109" s="28">
         <v>3830008640413</v>
       </c>
       <c r="F109" s="29" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G109" s="21" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="110" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A110" s="2"/>
       <c r="B110" s="37" t="s">
-        <v>268</v>
+        <v>375</v>
       </c>
       <c r="C110" s="35" t="s">
         <v>8</v>
@@ -4074,16 +4117,16 @@
         <v>3830008640413</v>
       </c>
       <c r="F110" s="29" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G110" s="21" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="111" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A111" s="3"/>
       <c r="B111" s="39" t="s">
-        <v>269</v>
+        <v>376</v>
       </c>
       <c r="C111" s="35" t="s">
         <v>8</v>
@@ -4095,16 +4138,16 @@
         <v>3830008640413</v>
       </c>
       <c r="F111" s="29" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G111" s="21" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="112" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A112" s="3"/>
       <c r="B112" s="39" t="s">
-        <v>270</v>
+        <v>377</v>
       </c>
       <c r="C112" s="35" t="s">
         <v>8</v>
@@ -4116,58 +4159,58 @@
         <v>3830008640413</v>
       </c>
       <c r="F112" s="29" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G112" s="21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="113" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A113" s="2"/>
       <c r="B113" s="37" t="s">
-        <v>271</v>
+        <v>378</v>
       </c>
       <c r="C113" s="35" t="s">
         <v>8</v>
       </c>
       <c r="D113" s="37" t="s">
-        <v>272</v>
+        <v>256</v>
       </c>
       <c r="E113" s="28">
         <v>3830008640413</v>
       </c>
       <c r="F113" s="29" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G113" s="19" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="114" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A114" s="2"/>
       <c r="B114" s="37" t="s">
-        <v>274</v>
+        <v>379</v>
       </c>
       <c r="C114" s="35" t="s">
         <v>8</v>
       </c>
       <c r="D114" s="37" t="s">
-        <v>275</v>
+        <v>258</v>
       </c>
       <c r="E114" s="28">
         <v>3830008640413</v>
       </c>
       <c r="F114" s="29" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G114" s="19" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="115" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A115" s="3"/>
       <c r="B115" s="39" t="s">
-        <v>276</v>
+        <v>380</v>
       </c>
       <c r="C115" s="35" t="s">
         <v>8</v>
@@ -4179,22 +4222,22 @@
         <v>3830008640413</v>
       </c>
       <c r="F115" s="29" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G115" s="21" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="116" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A116" s="3"/>
       <c r="B116" s="39" t="s">
-        <v>277</v>
+        <v>259</v>
       </c>
       <c r="C116" s="35" t="s">
         <v>8</v>
       </c>
       <c r="D116" s="39" t="s">
-        <v>278</v>
+        <v>260</v>
       </c>
       <c r="E116" s="28">
         <v>3830008640413</v>
@@ -4206,16 +4249,16 @@
         <v>48</v>
       </c>
     </row>
-    <row r="117" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A117" s="3"/>
       <c r="B117" s="39" t="s">
-        <v>279</v>
+        <v>261</v>
       </c>
       <c r="C117" s="35" t="s">
         <v>8</v>
       </c>
       <c r="D117" s="39" t="s">
-        <v>280</v>
+        <v>262</v>
       </c>
       <c r="E117" s="28">
         <v>3830008640413</v>
@@ -4227,16 +4270,16 @@
         <v>17</v>
       </c>
     </row>
-    <row r="118" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A118" s="3"/>
       <c r="B118" s="39" t="s">
-        <v>281</v>
+        <v>263</v>
       </c>
       <c r="C118" s="35" t="s">
         <v>8</v>
       </c>
       <c r="D118" s="39" t="s">
-        <v>282</v>
+        <v>264</v>
       </c>
       <c r="E118" s="28">
         <v>3830008640413</v>
@@ -4245,19 +4288,19 @@
         <v>10</v>
       </c>
       <c r="G118" s="21" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="119" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A119" s="3"/>
       <c r="B119" s="39" t="s">
-        <v>284</v>
+        <v>266</v>
       </c>
       <c r="C119" s="35" t="s">
         <v>8</v>
       </c>
       <c r="D119" s="39" t="s">
-        <v>285</v>
+        <v>267</v>
       </c>
       <c r="E119" s="28">
         <v>3830008640413</v>
@@ -4266,19 +4309,19 @@
         <v>10</v>
       </c>
       <c r="G119" s="21" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="120" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A120" s="3"/>
       <c r="B120" s="39" t="s">
-        <v>287</v>
+        <v>269</v>
       </c>
       <c r="C120" s="35" t="s">
         <v>8</v>
       </c>
       <c r="D120" s="39" t="s">
-        <v>288</v>
+        <v>270</v>
       </c>
       <c r="E120" s="28">
         <v>3830008640413</v>
@@ -4287,19 +4330,19 @@
         <v>10</v>
       </c>
       <c r="G120" s="21" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="121" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A121" s="2"/>
       <c r="B121" s="37" t="s">
-        <v>290</v>
+        <v>272</v>
       </c>
       <c r="C121" s="35" t="s">
         <v>8</v>
       </c>
       <c r="D121" s="37" t="s">
-        <v>291</v>
+        <v>273</v>
       </c>
       <c r="E121" s="28">
         <v>3830008640413</v>
@@ -4311,16 +4354,16 @@
         <v>23</v>
       </c>
     </row>
-    <row r="122" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A122" s="3"/>
       <c r="B122" s="39" t="s">
-        <v>292</v>
+        <v>274</v>
       </c>
       <c r="C122" s="35" t="s">
         <v>8</v>
       </c>
       <c r="D122" s="39" t="s">
-        <v>293</v>
+        <v>275</v>
       </c>
       <c r="E122" s="28">
         <v>3830008640413</v>
@@ -4332,16 +4375,16 @@
         <v>23</v>
       </c>
     </row>
-    <row r="123" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A123" s="3"/>
       <c r="B123" s="39" t="s">
-        <v>294</v>
+        <v>276</v>
       </c>
       <c r="C123" s="35" t="s">
         <v>8</v>
       </c>
       <c r="D123" s="39" t="s">
-        <v>295</v>
+        <v>277</v>
       </c>
       <c r="E123" s="28">
         <v>3830008640413</v>
@@ -4353,16 +4396,16 @@
         <v>23</v>
       </c>
     </row>
-    <row r="124" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A124" s="3"/>
       <c r="B124" s="39" t="s">
-        <v>296</v>
+        <v>278</v>
       </c>
       <c r="C124" s="35" t="s">
         <v>8</v>
       </c>
       <c r="D124" s="39" t="s">
-        <v>297</v>
+        <v>279</v>
       </c>
       <c r="E124" s="28">
         <v>3830008640413</v>
@@ -4371,19 +4414,19 @@
         <v>10</v>
       </c>
       <c r="G124" s="21" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="125" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A125" s="3"/>
       <c r="B125" s="39" t="s">
-        <v>299</v>
+        <v>281</v>
       </c>
       <c r="C125" s="35" t="s">
         <v>8</v>
       </c>
       <c r="D125" s="39" t="s">
-        <v>300</v>
+        <v>282</v>
       </c>
       <c r="E125" s="28">
         <v>3830008640413</v>
@@ -4392,19 +4435,19 @@
         <v>10</v>
       </c>
       <c r="G125" s="21" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="126" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A126" s="3"/>
       <c r="B126" s="39" t="s">
-        <v>302</v>
+        <v>284</v>
       </c>
       <c r="C126" s="35" t="s">
         <v>8</v>
       </c>
       <c r="D126" s="39" t="s">
-        <v>300</v>
+        <v>282</v>
       </c>
       <c r="E126" s="28">
         <v>3830008640413</v>
@@ -4413,19 +4456,19 @@
         <v>10</v>
       </c>
       <c r="G126" s="21" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="127" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A127" s="3"/>
       <c r="B127" s="39" t="s">
-        <v>303</v>
+        <v>285</v>
       </c>
       <c r="C127" s="35" t="s">
         <v>8</v>
       </c>
       <c r="D127" s="39" t="s">
-        <v>304</v>
+        <v>286</v>
       </c>
       <c r="E127" s="28">
         <v>3830008640413</v>
@@ -4434,34 +4477,34 @@
         <v>10</v>
       </c>
       <c r="G127" s="21" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="128" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A128" s="4"/>
       <c r="B128" s="40" t="s">
-        <v>306</v>
+        <v>347</v>
       </c>
       <c r="C128" s="35" t="s">
         <v>8</v>
       </c>
       <c r="D128" s="40" t="s">
-        <v>307</v>
+        <v>288</v>
       </c>
       <c r="E128" s="28">
         <v>3830008640413</v>
       </c>
       <c r="F128" s="29" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G128" s="22" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="129" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A129" s="3"/>
       <c r="B129" s="39" t="s">
-        <v>309</v>
+        <v>348</v>
       </c>
       <c r="C129" s="35" t="s">
         <v>8</v>
@@ -4473,253 +4516,253 @@
         <v>3830008640413</v>
       </c>
       <c r="F129" s="29" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G129" s="21" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="130" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A130" s="3"/>
       <c r="B130" s="39" t="s">
-        <v>310</v>
+        <v>349</v>
       </c>
       <c r="C130" s="35" t="s">
         <v>8</v>
       </c>
       <c r="D130" s="39" t="s">
-        <v>311</v>
+        <v>290</v>
       </c>
       <c r="E130" s="28">
         <v>3830008640413</v>
       </c>
       <c r="F130" s="29" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G130" s="21" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="131" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A131" s="3"/>
       <c r="B131" s="39" t="s">
-        <v>313</v>
+        <v>350</v>
       </c>
       <c r="C131" s="35" t="s">
         <v>8</v>
       </c>
       <c r="D131" s="39" t="s">
-        <v>314</v>
+        <v>292</v>
       </c>
       <c r="E131" s="28">
         <v>3830008640413</v>
       </c>
       <c r="F131" s="29" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G131" s="21" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="132" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A132" s="3"/>
       <c r="B132" s="39" t="s">
-        <v>316</v>
+        <v>351</v>
       </c>
       <c r="C132" s="35" t="s">
         <v>8</v>
       </c>
       <c r="D132" s="39" t="s">
-        <v>317</v>
+        <v>294</v>
       </c>
       <c r="E132" s="28">
         <v>3830008640413</v>
       </c>
       <c r="F132" s="29" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G132" s="21" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="133" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A133" s="3"/>
       <c r="B133" s="39" t="s">
-        <v>319</v>
+        <v>352</v>
       </c>
       <c r="C133" s="35" t="s">
         <v>8</v>
       </c>
       <c r="D133" s="39" t="s">
-        <v>320</v>
+        <v>296</v>
       </c>
       <c r="E133" s="28">
         <v>3830008640413</v>
       </c>
       <c r="F133" s="29" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G133" s="21" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="134" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A134" s="3"/>
       <c r="B134" s="39" t="s">
-        <v>322</v>
+        <v>353</v>
       </c>
       <c r="C134" s="35" t="s">
         <v>8</v>
       </c>
       <c r="D134" s="39" t="s">
-        <v>323</v>
+        <v>298</v>
       </c>
       <c r="E134" s="28">
         <v>3830008640413</v>
       </c>
       <c r="F134" s="29" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G134" s="21" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="135" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A135" s="3"/>
       <c r="B135" s="39" t="s">
-        <v>325</v>
+        <v>354</v>
       </c>
       <c r="C135" s="35" t="s">
         <v>8</v>
       </c>
       <c r="D135" s="39" t="s">
-        <v>326</v>
+        <v>300</v>
       </c>
       <c r="E135" s="28">
         <v>3830008640413</v>
       </c>
       <c r="F135" s="29" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G135" s="21" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="136" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A136" s="5"/>
       <c r="B136" s="41" t="s">
-        <v>327</v>
+        <v>355</v>
       </c>
       <c r="C136" s="35" t="s">
         <v>8</v>
       </c>
       <c r="D136" s="41" t="s">
-        <v>328</v>
+        <v>301</v>
       </c>
       <c r="E136" s="28">
         <v>3830008640413</v>
       </c>
       <c r="F136" s="29" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G136" s="23" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="137" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A137" s="5"/>
       <c r="B137" s="41" t="s">
-        <v>329</v>
+        <v>356</v>
       </c>
       <c r="C137" s="35" t="s">
         <v>8</v>
       </c>
       <c r="D137" s="41" t="s">
-        <v>330</v>
+        <v>302</v>
       </c>
       <c r="E137" s="28">
         <v>3830008640413</v>
       </c>
       <c r="F137" s="29" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G137" s="23" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="138" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A138" s="5"/>
       <c r="B138" s="41" t="s">
-        <v>331</v>
+        <v>357</v>
       </c>
       <c r="C138" s="35" t="s">
         <v>8</v>
       </c>
       <c r="D138" s="41" t="s">
-        <v>332</v>
+        <v>303</v>
       </c>
       <c r="E138" s="28">
         <v>3830008640413</v>
       </c>
       <c r="F138" s="29" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G138" s="23" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="139" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A139" s="6"/>
       <c r="B139" s="42" t="s">
-        <v>334</v>
+        <v>305</v>
       </c>
       <c r="C139" s="35" t="s">
         <v>8</v>
       </c>
       <c r="D139" s="39" t="s">
-        <v>335</v>
+        <v>306</v>
       </c>
       <c r="E139" s="28">
         <v>3830008640413</v>
       </c>
       <c r="F139" s="29" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G139" s="21" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="140" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A140" s="6"/>
       <c r="B140" s="42" t="s">
-        <v>337</v>
+        <v>308</v>
       </c>
       <c r="C140" s="35" t="s">
         <v>8</v>
       </c>
       <c r="D140" s="39" t="s">
-        <v>338</v>
+        <v>309</v>
       </c>
       <c r="E140" s="28">
         <v>3830008640413</v>
       </c>
       <c r="F140" s="29" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G140" s="21" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="141" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A141" s="6"/>
       <c r="B141" s="42" t="s">
-        <v>340</v>
+        <v>311</v>
       </c>
       <c r="C141" s="35" t="s">
         <v>8</v>
       </c>
       <c r="D141" s="43" t="s">
-        <v>341</v>
+        <v>312</v>
       </c>
       <c r="E141" s="28">
         <v>3830008640413</v>
@@ -4728,19 +4771,19 @@
         <v>10</v>
       </c>
       <c r="G141" s="24" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="142" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A142" s="6"/>
       <c r="B142" s="42" t="s">
-        <v>343</v>
+        <v>314</v>
       </c>
       <c r="C142" s="35" t="s">
         <v>8</v>
       </c>
       <c r="D142" s="43" t="s">
-        <v>341</v>
+        <v>312</v>
       </c>
       <c r="E142" s="28">
         <v>3830008640413</v>
@@ -4749,19 +4792,19 @@
         <v>10</v>
       </c>
       <c r="G142" s="24" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="143" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A143" s="6"/>
       <c r="B143" s="42" t="s">
-        <v>344</v>
+        <v>315</v>
       </c>
       <c r="C143" s="35" t="s">
         <v>8</v>
       </c>
       <c r="D143" s="43" t="s">
-        <v>341</v>
+        <v>312</v>
       </c>
       <c r="E143" s="28">
         <v>3830008640413</v>
@@ -4770,19 +4813,19 @@
         <v>10</v>
       </c>
       <c r="G143" s="24" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="144" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A144" s="6"/>
       <c r="B144" s="42" t="s">
-        <v>345</v>
+        <v>316</v>
       </c>
       <c r="C144" s="35" t="s">
         <v>8</v>
       </c>
       <c r="D144" s="43" t="s">
-        <v>346</v>
+        <v>317</v>
       </c>
       <c r="E144" s="28">
         <v>3830008640413</v>
@@ -4791,19 +4834,19 @@
         <v>10</v>
       </c>
       <c r="G144" s="24" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="145" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A145" s="6"/>
       <c r="B145" s="42" t="s">
-        <v>348</v>
+        <v>319</v>
       </c>
       <c r="C145" s="35" t="s">
         <v>8</v>
       </c>
       <c r="D145" s="43" t="s">
-        <v>349</v>
+        <v>320</v>
       </c>
       <c r="E145" s="28">
         <v>3830008640413</v>
@@ -4812,19 +4855,19 @@
         <v>10</v>
       </c>
       <c r="G145" s="24" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="146" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A146" s="6"/>
       <c r="B146" s="42" t="s">
-        <v>351</v>
+        <v>322</v>
       </c>
       <c r="C146" s="35" t="s">
         <v>8</v>
       </c>
       <c r="D146" s="43" t="s">
-        <v>352</v>
+        <v>323</v>
       </c>
       <c r="E146" s="28">
         <v>3830008640413</v>
@@ -4833,19 +4876,19 @@
         <v>10</v>
       </c>
       <c r="G146" s="24" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="147" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A147" s="6"/>
       <c r="B147" s="42" t="s">
-        <v>354</v>
+        <v>325</v>
       </c>
       <c r="C147" s="35" t="s">
         <v>8</v>
       </c>
       <c r="D147" s="43" t="s">
-        <v>355</v>
+        <v>326</v>
       </c>
       <c r="E147" s="28">
         <v>3830008640413</v>
@@ -4854,31 +4897,31 @@
         <v>10</v>
       </c>
       <c r="G147" s="24" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="148" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A148" s="6"/>
       <c r="B148" s="42" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="C148" s="35" t="s">
         <v>8</v>
       </c>
       <c r="D148" s="43" t="s">
-        <v>349</v>
+        <v>320</v>
       </c>
       <c r="E148" s="28">
         <v>3830008640413</v>
       </c>
       <c r="F148" s="29" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G148" s="24" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="149" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A149" s="6"/>
       <c r="B149" s="42" t="s">
         <v>359</v>
@@ -4887,43 +4930,43 @@
         <v>8</v>
       </c>
       <c r="D149" s="43" t="s">
-        <v>360</v>
+        <v>329</v>
       </c>
       <c r="E149" s="28">
         <v>3830008640413</v>
       </c>
       <c r="F149" s="29" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G149" s="24" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="150" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A150" s="6"/>
       <c r="B150" s="42" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C150" s="35" t="s">
         <v>8</v>
       </c>
       <c r="D150" s="43" t="s">
-        <v>363</v>
+        <v>331</v>
       </c>
       <c r="E150" s="28">
         <v>3830008640413</v>
       </c>
       <c r="F150" s="29" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G150" s="24" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="151" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A151" s="6"/>
       <c r="B151" s="42" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="C151" s="35" t="s">
         <v>8</v>
@@ -4935,43 +4978,43 @@
         <v>3830008640413</v>
       </c>
       <c r="F151" s="29" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G151" s="24" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="152" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A152" s="6"/>
       <c r="B152" s="42" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="C152" s="35" t="s">
         <v>8</v>
       </c>
       <c r="D152" s="43" t="s">
-        <v>367</v>
+        <v>333</v>
       </c>
       <c r="E152" s="28">
         <v>3830008640413</v>
       </c>
       <c r="F152" s="29" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G152" s="24" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="153" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A153" s="6"/>
       <c r="B153" s="42" t="s">
-        <v>369</v>
+        <v>335</v>
       </c>
       <c r="C153" s="35" t="s">
         <v>8</v>
       </c>
       <c r="D153" s="43" t="s">
-        <v>367</v>
+        <v>333</v>
       </c>
       <c r="E153" s="28">
         <v>3830008640413</v>
@@ -4980,19 +5023,19 @@
         <v>10</v>
       </c>
       <c r="G153" s="24" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="154" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A154" s="6"/>
       <c r="B154" s="42" t="s">
-        <v>370</v>
+        <v>336</v>
       </c>
       <c r="C154" s="35" t="s">
         <v>8</v>
       </c>
       <c r="D154" s="43" t="s">
-        <v>371</v>
+        <v>337</v>
       </c>
       <c r="E154" s="28">
         <v>3830008640413</v>
@@ -5001,19 +5044,19 @@
         <v>10</v>
       </c>
       <c r="G154" s="24" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="155" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A155" s="7"/>
       <c r="B155" s="42" t="s">
-        <v>373</v>
+        <v>339</v>
       </c>
       <c r="C155" s="35" t="s">
         <v>8</v>
       </c>
       <c r="D155" s="44" t="s">
-        <v>374</v>
+        <v>340</v>
       </c>
       <c r="E155" s="28">
         <v>3830008640413</v>
@@ -5022,13 +5065,13 @@
         <v>10</v>
       </c>
       <c r="G155" s="25" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="156" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A156" s="8"/>
       <c r="B156" s="45" t="s">
-        <v>376</v>
+        <v>342</v>
       </c>
       <c r="C156" s="35" t="s">
         <v>8</v>
@@ -5046,11 +5089,11 @@
         <v>57</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F157" s="32"/>
       <c r="G157" s="10"/>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A158" s="11"/>
       <c r="B158" s="33"/>
       <c r="C158" s="32"/>
@@ -5059,7 +5102,7 @@
       <c r="F158" s="32"/>
       <c r="G158" s="10"/>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A159" s="11"/>
       <c r="B159" s="33"/>
       <c r="C159" s="32"/>
@@ -5068,7 +5111,7 @@
       <c r="F159" s="32"/>
       <c r="G159" s="10"/>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A160" s="11"/>
       <c r="B160" s="33"/>
       <c r="C160" s="32"/>
@@ -5077,7 +5120,7 @@
       <c r="F160" s="32"/>
       <c r="G160" s="10"/>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A161" s="11"/>
       <c r="B161" s="33"/>
       <c r="C161" s="32"/>
@@ -5086,7 +5129,7 @@
       <c r="F161" s="32"/>
       <c r="G161" s="10"/>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A162" s="11"/>
       <c r="B162" s="33"/>
       <c r="C162" s="32"/>
@@ -5095,7 +5138,7 @@
       <c r="F162" s="32"/>
       <c r="G162" s="10"/>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A163" s="11"/>
       <c r="B163" s="33"/>
       <c r="C163" s="32"/>
@@ -5104,7 +5147,7 @@
       <c r="F163" s="32"/>
       <c r="G163" s="10"/>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A164" s="11"/>
       <c r="B164" s="33"/>
       <c r="C164" s="32"/>
@@ -5113,7 +5156,7 @@
       <c r="F164" s="32"/>
       <c r="G164" s="10"/>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A165" s="11"/>
       <c r="B165" s="33"/>
       <c r="C165" s="32"/>
@@ -5131,24 +5174,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>